<commit_message>
change name in pom.xml
</commit_message>
<xml_diff>
--- a/RestfulAPITest/Http_Request_workbook_Data.xlsx
+++ b/RestfulAPITest/Http_Request_workbook_Data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>2015-09-17 10:48:28</t>
+  </si>
+  <si>
+    <t>2015-09-17 11:38:23</t>
+  </si>
+  <si>
+    <t>2015-09-17 11:38:25</t>
   </si>
 </sst>
 </file>
@@ -819,10 +825,10 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">

</xml_diff>